<commit_message>
agenda domingo en otra rama
</commit_message>
<xml_diff>
--- a/AGENDA.xlsx
+++ b/AGENDA.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>GIT</t>
   </si>
   <si>
-    <t>17/11/2022</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
@@ -54,6 +51,12 @@
   </si>
   <si>
     <t>INGLES</t>
+  </si>
+  <si>
+    <t>18/11/2022</t>
+  </si>
+  <si>
+    <t>C#</t>
   </si>
 </sst>
 </file>
@@ -69,7 +72,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,6 +91,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -101,12 +110,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -132,7 +142,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:H22" totalsRowShown="0">
   <autoFilter ref="A1:H22"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="17/11/2022"/>
+    <tableColumn id="1" name="18/11/2022"/>
     <tableColumn id="8" name="0" dataDxfId="0"/>
     <tableColumn id="2" name="10"/>
     <tableColumn id="3" name="20"/>
@@ -410,8 +420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H18" activeCellId="5" sqref="C18 D18 E18 F18 G18 H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,28 +433,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -491,13 +501,18 @@
       <c r="A10">
         <v>13</v>
       </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>14</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -541,13 +556,21 @@
       <c r="A18">
         <v>21</v>
       </c>
+      <c r="C18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>22</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>

</xml_diff>